<commit_message>
Uppfærsla á excel skjali #135
</commit_message>
<xml_diff>
--- a/Vinnusvæði/Verkþáttur 4/Review/2022-01-25/Samanburður 2013 og 2022 IOBS.xlsx
+++ b/Vinnusvæði/Verkþáttur 4/Review/2022-01-25/Samanburður 2013 og 2022 IOBS.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Staðlaráð\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\fintech\IST-FUT-FMTH\Vinnusvæði\Verkþáttur 4\Review\2022-01-25\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A588C4C-CB45-42C0-872A-04B0212C0FC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC06A564-C2AE-4658-B37E-72E5A1FCB43A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9DBE8D8B-B416-4EA5-B2AC-D8D20FAD8234}"/>
+    <workbookView xWindow="15960" yWindow="180" windowWidth="31350" windowHeight="17220" activeTab="5" xr2:uid="{9DBE8D8B-B416-4EA5-B2AC-D8D20FAD8234}"/>
   </bookViews>
   <sheets>
     <sheet name="QueryClaim" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="942" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="974" uniqueCount="288">
   <si>
     <t>IOBS 3.0</t>
   </si>
@@ -888,6 +888,21 @@
   </si>
   <si>
     <t>//Currency.Rate = 1;</t>
+  </si>
+  <si>
+    <t>YAML</t>
+  </si>
+  <si>
+    <t>DEL</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>SecondaryCollectionTemplateCode og SecondaryCollectionClaimTemplateId</t>
+  </si>
+  <si>
+    <t>Legal collection fer út</t>
   </si>
 </sst>
 </file>
@@ -990,7 +1005,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1012,6 +1027,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -1329,26 +1345,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{633905DF-87A6-41D6-8799-89CE7F748DC3}">
-  <dimension ref="B2:E104"/>
+  <dimension ref="A2:E104"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="C86" sqref="C86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="9.140625" style="13"/>
     <col min="2" max="2" width="81.85546875" customWidth="1"/>
     <col min="3" max="3" width="83.5703125" customWidth="1"/>
     <col min="5" max="5" width="89.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" s="12" t="s">
         <v>96</v>
       </c>
       <c r="C2" s="12"/>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
@@ -1356,7 +1373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
@@ -1364,7 +1381,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>3</v>
       </c>
@@ -1378,7 +1395,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>4</v>
       </c>
@@ -1386,7 +1403,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>5</v>
       </c>
@@ -1397,7 +1414,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>6</v>
       </c>
@@ -1408,7 +1425,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>7</v>
       </c>
@@ -1419,7 +1436,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C10" s="4" t="s">
         <v>99</v>
       </c>
@@ -1427,7 +1444,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>8</v>
       </c>
@@ -1441,7 +1458,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>9</v>
       </c>
@@ -1455,7 +1472,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>10</v>
       </c>
@@ -1466,7 +1483,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>11</v>
       </c>
@@ -1477,7 +1494,10 @@
         <v>125</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="s">
+        <v>283</v>
+      </c>
       <c r="B15" t="s">
         <v>12</v>
       </c>
@@ -1488,7 +1508,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>13</v>
       </c>
@@ -1496,7 +1516,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>14</v>
       </c>
@@ -1504,7 +1524,10 @@
         <v>103</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
+        <v>284</v>
+      </c>
       <c r="C18" s="4" t="s">
         <v>279</v>
       </c>
@@ -1512,7 +1535,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>15</v>
       </c>
@@ -1520,7 +1543,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>16</v>
       </c>
@@ -1534,7 +1557,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>17</v>
       </c>
@@ -1548,7 +1571,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>18</v>
       </c>
@@ -1562,7 +1585,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>19</v>
       </c>
@@ -1576,7 +1599,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>20</v>
       </c>
@@ -1590,7 +1613,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>21</v>
       </c>
@@ -1604,7 +1627,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>22</v>
       </c>
@@ -1612,7 +1635,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>23</v>
       </c>
@@ -1626,7 +1649,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>24</v>
       </c>
@@ -1637,7 +1660,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>25</v>
       </c>
@@ -1645,7 +1668,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>26</v>
       </c>
@@ -1656,7 +1679,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>27</v>
       </c>
@@ -1664,7 +1687,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>28</v>
       </c>
@@ -1866,7 +1889,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>45</v>
       </c>
@@ -1880,7 +1903,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>46</v>
       </c>
@@ -1888,7 +1911,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>47</v>
       </c>
@@ -1896,7 +1919,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>48</v>
       </c>
@@ -1910,7 +1933,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>49</v>
       </c>
@@ -1924,7 +1947,10 @@
         <v>155</v>
       </c>
     </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="13" t="s">
+        <v>285</v>
+      </c>
       <c r="B54" t="s">
         <v>50</v>
       </c>
@@ -1935,7 +1961,10 @@
         <v>125</v>
       </c>
     </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="13" t="s">
+        <v>285</v>
+      </c>
       <c r="B55" t="s">
         <v>51</v>
       </c>
@@ -1946,7 +1975,10 @@
         <v>125</v>
       </c>
     </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="13" t="s">
+        <v>285</v>
+      </c>
       <c r="B56" t="s">
         <v>52</v>
       </c>
@@ -1957,7 +1989,10 @@
         <v>125</v>
       </c>
     </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="13" t="s">
+        <v>285</v>
+      </c>
       <c r="B57" t="s">
         <v>53</v>
       </c>
@@ -1968,7 +2003,10 @@
         <v>125</v>
       </c>
     </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="13" t="s">
+        <v>285</v>
+      </c>
       <c r="B58" t="s">
         <v>54</v>
       </c>
@@ -1979,7 +2017,10 @@
         <v>125</v>
       </c>
     </row>
-    <row r="59" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="13" t="s">
+        <v>285</v>
+      </c>
       <c r="B59" t="s">
         <v>55</v>
       </c>
@@ -1990,7 +2031,10 @@
         <v>125</v>
       </c>
     </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="13" t="s">
+        <v>285</v>
+      </c>
       <c r="B60" t="s">
         <v>56</v>
       </c>
@@ -2001,7 +2045,10 @@
         <v>125</v>
       </c>
     </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="13" t="s">
+        <v>285</v>
+      </c>
       <c r="B61" t="s">
         <v>57</v>
       </c>
@@ -2012,7 +2059,10 @@
         <v>125</v>
       </c>
     </row>
-    <row r="62" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="13" t="s">
+        <v>285</v>
+      </c>
       <c r="B62" t="s">
         <v>58</v>
       </c>
@@ -2023,7 +2073,10 @@
         <v>125</v>
       </c>
     </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="13" t="s">
+        <v>285</v>
+      </c>
       <c r="B63" t="s">
         <v>59</v>
       </c>
@@ -2034,7 +2087,10 @@
         <v>125</v>
       </c>
     </row>
-    <row r="64" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="13" t="s">
+        <v>285</v>
+      </c>
       <c r="B64" t="s">
         <v>60</v>
       </c>
@@ -2045,7 +2101,10 @@
         <v>125</v>
       </c>
     </row>
-    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="13" t="s">
+        <v>285</v>
+      </c>
       <c r="B65" t="s">
         <v>61</v>
       </c>
@@ -2056,7 +2115,10 @@
         <v>125</v>
       </c>
     </row>
-    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="13" t="s">
+        <v>285</v>
+      </c>
       <c r="B66" t="s">
         <v>62</v>
       </c>
@@ -2067,7 +2129,10 @@
         <v>125</v>
       </c>
     </row>
-    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="13" t="s">
+        <v>285</v>
+      </c>
       <c r="B67" t="s">
         <v>63</v>
       </c>
@@ -2078,7 +2143,10 @@
         <v>125</v>
       </c>
     </row>
-    <row r="68" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="13" t="s">
+        <v>285</v>
+      </c>
       <c r="B68" t="s">
         <v>64</v>
       </c>
@@ -2089,7 +2157,10 @@
         <v>125</v>
       </c>
     </row>
-    <row r="69" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="13" t="s">
+        <v>285</v>
+      </c>
       <c r="B69" t="s">
         <v>65</v>
       </c>
@@ -2097,7 +2168,10 @@
         <v>125</v>
       </c>
     </row>
-    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="13" t="s">
+        <v>285</v>
+      </c>
       <c r="B70" t="s">
         <v>66</v>
       </c>
@@ -2105,7 +2179,10 @@
         <v>125</v>
       </c>
     </row>
-    <row r="71" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="13" t="s">
+        <v>285</v>
+      </c>
       <c r="B71" t="s">
         <v>67</v>
       </c>
@@ -2116,7 +2193,10 @@
         <v>125</v>
       </c>
     </row>
-    <row r="72" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="13" t="s">
+        <v>285</v>
+      </c>
       <c r="B72" t="s">
         <v>68</v>
       </c>
@@ -2127,7 +2207,10 @@
         <v>125</v>
       </c>
     </row>
-    <row r="73" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="13" t="s">
+        <v>285</v>
+      </c>
       <c r="B73" t="s">
         <v>69</v>
       </c>
@@ -2138,7 +2221,10 @@
         <v>125</v>
       </c>
     </row>
-    <row r="74" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="13" t="s">
+        <v>285</v>
+      </c>
       <c r="B74" t="s">
         <v>70</v>
       </c>
@@ -2149,7 +2235,10 @@
         <v>125</v>
       </c>
     </row>
-    <row r="75" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="13" t="s">
+        <v>285</v>
+      </c>
       <c r="B75" t="s">
         <v>71</v>
       </c>
@@ -2160,7 +2249,10 @@
         <v>125</v>
       </c>
     </row>
-    <row r="76" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="13" t="s">
+        <v>285</v>
+      </c>
       <c r="B76" t="s">
         <v>72</v>
       </c>
@@ -2171,7 +2263,10 @@
         <v>125</v>
       </c>
     </row>
-    <row r="77" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="13" t="s">
+        <v>285</v>
+      </c>
       <c r="B77" t="s">
         <v>73</v>
       </c>
@@ -2182,7 +2277,10 @@
         <v>125</v>
       </c>
     </row>
-    <row r="78" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="13" t="s">
+        <v>285</v>
+      </c>
       <c r="B78" t="s">
         <v>74</v>
       </c>
@@ -2193,7 +2291,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="79" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
         <v>75</v>
       </c>
@@ -2201,7 +2299,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="80" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
         <v>76</v>
       </c>
@@ -2211,8 +2309,11 @@
       <c r="D80" s="5" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="81" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E80" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
         <v>77</v>
       </c>
@@ -2223,7 +2324,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="82" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
         <v>78</v>
       </c>
@@ -2234,7 +2335,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="83" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
         <v>79</v>
       </c>
@@ -2245,7 +2346,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="84" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
         <v>80</v>
       </c>
@@ -2256,7 +2357,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="85" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
         <v>81</v>
       </c>
@@ -2267,7 +2368,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="86" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
         <v>82</v>
       </c>
@@ -2278,7 +2379,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="87" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
         <v>83</v>
       </c>
@@ -2289,7 +2390,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="88" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
         <v>84</v>
       </c>
@@ -2300,7 +2401,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="89" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
         <v>85</v>
       </c>
@@ -2311,7 +2412,10 @@
         <v>118</v>
       </c>
     </row>
-    <row r="90" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" s="13" t="s">
+        <v>285</v>
+      </c>
       <c r="B90" t="s">
         <v>86</v>
       </c>
@@ -2321,8 +2425,11 @@
       <c r="D90" s="5" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="91" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E90" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
         <v>87</v>
       </c>
@@ -2333,7 +2440,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="92" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
         <v>88</v>
       </c>
@@ -2344,7 +2451,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="93" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
         <v>89</v>
       </c>
@@ -2355,7 +2462,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="94" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
         <v>90</v>
       </c>
@@ -2366,7 +2473,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="95" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
         <v>91</v>
       </c>
@@ -2377,7 +2484,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="96" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
         <v>92</v>
       </c>
@@ -2466,8 +2573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3249E01-1138-4B32-9CF1-2F09083F4474}">
   <dimension ref="B2:E79"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18:D18"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3349,7 +3456,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7569136C-1755-44CC-8CB8-7F6C3204D25A}">
   <dimension ref="B2:E84"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A46" workbookViewId="0">
       <selection activeCell="C18" sqref="C18:D18"/>
     </sheetView>
   </sheetViews>
@@ -4285,8 +4392,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4799C5DE-DF6E-46DA-A3CB-E59A285E9DA9}">
   <dimension ref="B2:E40"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18:C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4806,9 +4913,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9F13751-6B3C-4CAF-8671-2D17A637C6CE}">
-  <dimension ref="B2:Q15"/>
+  <dimension ref="A2:Q15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4819,7 +4928,7 @@
     <col min="17" max="17" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>252</v>
       </c>
@@ -4830,12 +4939,12 @@
         <v>271</v>
       </c>
     </row>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="L3" s="1" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>253</v>
       </c>
@@ -4852,7 +4961,7 @@
       <c r="P4" s="8"/>
       <c r="Q4" s="8"/>
     </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>254</v>
       </c>
@@ -4869,17 +4978,17 @@
       <c r="P5" s="9"/>
       <c r="Q5" s="9"/>
     </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>257</v>
       </c>
@@ -4890,7 +4999,10 @@
         <v>275</v>
       </c>
     </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
+        <v>285</v>
+      </c>
       <c r="B9" t="s">
         <v>258</v>
       </c>
@@ -4901,7 +5013,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>259</v>
       </c>
@@ -4912,7 +5024,10 @@
         <v>277</v>
       </c>
     </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
+        <v>285</v>
+      </c>
       <c r="B11" t="s">
         <v>260</v>
       </c>
@@ -4923,7 +5038,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>261</v>
       </c>
@@ -4934,17 +5049,17 @@
         <v>278</v>
       </c>
     </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>264</v>
       </c>

</xml_diff>

<commit_message>
#135 Updated according to the Excel document from Sigurði Alskil. Patch reworked according to Asgeir comment. Missing fields added and amount, value and % presented as double.
Validate using SwaggerHub https://app.swaggerhub.com/apis/Openbanking.is/iobws-3_0_domestic_claims/3.0#/
</commit_message>
<xml_diff>
--- a/Vinnusvæði/Verkþáttur 4/Review/2022-01-25/Samanburður 2013 og 2022 IOBS.xlsx
+++ b/Vinnusvæði/Verkþáttur 4/Review/2022-01-25/Samanburður 2013 og 2022 IOBS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\fintech\IST-FUT-FMTH\Vinnusvæði\Verkþáttur 4\Review\2022-01-25\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC06A564-C2AE-4658-B37E-72E5A1FCB43A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9899CC2E-7B3A-4528-A5FB-7289786EFFC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15960" yWindow="180" windowWidth="31350" windowHeight="17220" activeTab="5" xr2:uid="{9DBE8D8B-B416-4EA5-B2AC-D8D20FAD8234}"/>
+    <workbookView xWindow="20340" yWindow="3720" windowWidth="31350" windowHeight="17220" xr2:uid="{9DBE8D8B-B416-4EA5-B2AC-D8D20FAD8234}"/>
   </bookViews>
   <sheets>
     <sheet name="QueryClaim" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="974" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1001" uniqueCount="300">
   <si>
     <t>IOBS 3.0</t>
   </si>
@@ -903,13 +903,49 @@
   </si>
   <si>
     <t>Legal collection fer út</t>
+  </si>
+  <si>
+    <t>Enum</t>
+  </si>
+  <si>
+    <t>Leiðrétt</t>
+  </si>
+  <si>
+    <t>double</t>
+  </si>
+  <si>
+    <t>Leiðrétt, enum</t>
+  </si>
+  <si>
+    <t>claimState</t>
+  </si>
+  <si>
+    <t>claimStatus</t>
+  </si>
+  <si>
+    <t>Nýtt enum</t>
+  </si>
+  <si>
+    <t>Komið inn</t>
+  </si>
+  <si>
+    <t>Sjá word skjal</t>
+  </si>
+  <si>
+    <t>Tekið út</t>
+  </si>
+  <si>
+    <t>Lagað</t>
+  </si>
+  <si>
+    <t>Sleppt</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -942,6 +978,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1005,7 +1047,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1024,10 +1066,31 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -1345,1218 +1408,1264 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{633905DF-87A6-41D6-8799-89CE7F748DC3}">
-  <dimension ref="A2:E104"/>
+  <dimension ref="A2:F104"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="C86" sqref="C86"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E96" sqref="E96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="13"/>
-    <col min="2" max="2" width="81.85546875" customWidth="1"/>
-    <col min="3" max="3" width="83.5703125" customWidth="1"/>
-    <col min="5" max="5" width="89.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="12"/>
+    <col min="2" max="2" width="81.85546875" style="15" customWidth="1"/>
+    <col min="3" max="3" width="75.7109375" style="15" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="15"/>
+    <col min="5" max="5" width="46" style="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="12" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="C2" s="12"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
+      <c r="C2" s="14"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="16" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="16" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="E5" s="5" t="s">
+      <c r="D5" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="E5" s="18" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+      <c r="F5" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="15" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="19" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="19" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="19" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C10" s="4" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C10" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="19" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="D11" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="E11" s="15" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="E12" t="s">
+      <c r="D12" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="E12" s="15" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="15" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
+    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B14" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="15" t="s">
         <v>231</v>
       </c>
-      <c r="D14" s="5" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="13" t="s">
+      <c r="D14" s="18" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="12" t="s">
         <v>283</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="15" t="s">
         <v>229</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="E15" s="18" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
+      <c r="F15" s="15" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="15" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="13" t="s">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="12" t="s">
         <v>284</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="19" t="s">
         <v>279</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="19" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
+    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B19" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="15" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="15" t="s">
         <v>127</v>
       </c>
-      <c r="D20" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="E20" t="s">
+      <c r="D20" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="E20" s="15" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="15" t="s">
         <v>128</v>
       </c>
-      <c r="D21" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="E21" t="s">
+      <c r="D21" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="E21" s="15" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="15" t="s">
         <v>134</v>
       </c>
-      <c r="D22" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="E22" t="s">
+      <c r="D22" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="E22" s="15" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
+    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B23" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="C23" s="18" t="s">
         <v>135</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D23" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="E23" s="5" t="s">
+      <c r="E23" s="18" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
+      <c r="F23" s="20" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B24" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="15" t="s">
         <v>138</v>
       </c>
-      <c r="D24" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="E24" t="s">
+      <c r="D24" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="E24" s="15" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="15" t="s">
         <v>139</v>
       </c>
-      <c r="D25" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="E25" t="s">
+      <c r="D25" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="E25" s="15" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B26" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="15" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B27" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="D27" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="E27" t="s">
+      <c r="D27" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="E27" s="15" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B28" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="15" t="s">
         <v>141</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="D28" s="19" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
+    <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B29" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="15" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
+    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B30" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="15" t="s">
         <v>235</v>
       </c>
-      <c r="D30" s="3" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
+      <c r="D30" s="17" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B31" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="15" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B32" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="D32" s="19" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
+    <row r="33" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B33" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="15" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B34" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="15" t="s">
         <v>144</v>
       </c>
-      <c r="D34" s="3" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
+      <c r="D34" s="17" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B35" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" s="15" t="s">
         <v>147</v>
       </c>
-      <c r="D35" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="E35" t="s">
+      <c r="D35" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="E35" s="15" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B36" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="15" t="s">
         <v>148</v>
       </c>
-      <c r="D36" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="E36" t="s">
+      <c r="D36" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="E36" s="15" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
+    <row r="37" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B37" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="15" t="s">
         <v>149</v>
       </c>
-      <c r="D37" s="5" t="s">
+      <c r="D37" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="E37" s="5" t="s">
+      <c r="E37" s="18" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
+      <c r="F37" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B38" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="15" t="s">
         <v>150</v>
       </c>
-      <c r="D38" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="E38" t="s">
+      <c r="D38" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="E38" s="15" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B39" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="D39" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="E39" t="s">
+      <c r="D39" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="E39" s="15" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B40" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C40" s="15" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B41" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41" s="15" t="s">
         <v>152</v>
       </c>
-      <c r="D41" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="E41" t="s">
+      <c r="D41" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="E41" s="15" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B42" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" s="15" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
+    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B43" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C43" s="15" t="s">
         <v>156</v>
       </c>
-      <c r="D43" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="E43" t="s">
+      <c r="D43" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="E43" s="15" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
+    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B44" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44" s="15" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
+    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B45" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C45" s="15" t="s">
         <v>157</v>
       </c>
-      <c r="D45" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="E45" t="s">
+      <c r="D45" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="E45" s="15" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B46" t="s">
+    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B46" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C46" s="15" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
+    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B47" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C47" s="15" t="s">
         <v>158</v>
       </c>
-      <c r="D47" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="E47" t="s">
+      <c r="D47" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="E47" s="15" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B48" t="s">
+    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B48" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C48" s="15" t="s">
         <v>159</v>
       </c>
-      <c r="D48" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="E48" t="s">
+      <c r="D48" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="E48" s="15" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B49" t="s">
+      <c r="B49" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C49" s="15" t="s">
         <v>161</v>
       </c>
-      <c r="D49" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="E49" t="s">
+      <c r="D49" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="E49" s="15" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B50" t="s">
+      <c r="B50" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C50" s="15" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B51" t="s">
+      <c r="B51" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C51" s="15" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B52" t="s">
+      <c r="B52" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C52" s="15" t="s">
         <v>163</v>
       </c>
-      <c r="D52" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="E52" t="s">
+      <c r="D52" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="E52" s="15" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
+      <c r="B53" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C53" s="15" t="s">
         <v>164</v>
       </c>
-      <c r="D53" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="E53" t="s">
+      <c r="D53" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="E53" s="15" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="13" t="s">
+      <c r="A54" s="12" t="s">
         <v>285</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B54" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C54" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="D54" s="5" t="s">
+      <c r="D54" s="18" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="13" t="s">
+      <c r="A55" s="12" t="s">
         <v>285</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C55" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="D55" s="5" t="s">
+      <c r="D55" s="18" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="13" t="s">
+      <c r="A56" s="12" t="s">
         <v>285</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B56" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C56" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="D56" s="5" t="s">
+      <c r="D56" s="18" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="13" t="s">
+      <c r="A57" s="12" t="s">
         <v>285</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B57" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C57" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="D57" s="5" t="s">
+      <c r="D57" s="18" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="13" t="s">
+      <c r="A58" s="12" t="s">
         <v>285</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B58" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C58" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="D58" s="5" t="s">
+      <c r="D58" s="18" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="13" t="s">
+      <c r="A59" s="12" t="s">
         <v>285</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B59" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C59" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="D59" s="5" t="s">
+      <c r="D59" s="18" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="13" t="s">
+      <c r="A60" s="12" t="s">
         <v>285</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B60" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C60" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="D60" s="5" t="s">
+      <c r="D60" s="18" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="13" t="s">
+      <c r="A61" s="12" t="s">
         <v>285</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B61" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C61" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="D61" s="5" t="s">
+      <c r="D61" s="18" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="13" t="s">
+      <c r="A62" s="12" t="s">
         <v>285</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B62" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C62" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="D62" s="5" t="s">
+      <c r="D62" s="18" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="13" t="s">
+      <c r="A63" s="12" t="s">
         <v>285</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B63" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C63" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="D63" s="5" t="s">
+      <c r="D63" s="18" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="13" t="s">
+      <c r="A64" s="12" t="s">
         <v>285</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B64" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C64" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="D64" s="5" t="s">
+      <c r="D64" s="18" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="13" t="s">
+      <c r="A65" s="12" t="s">
         <v>285</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B65" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C65" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="D65" s="5" t="s">
+      <c r="D65" s="18" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="13" t="s">
+      <c r="A66" s="12" t="s">
         <v>285</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B66" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C66" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="D66" s="5" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="13" t="s">
+      <c r="D66" s="18" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A67" s="12" t="s">
         <v>285</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B67" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C67" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="D67" s="5" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="13" t="s">
+      <c r="D67" s="18" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A68" s="12" t="s">
         <v>285</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B68" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="C68" t="s">
+      <c r="C68" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="D68" s="5" t="s">
+      <c r="D68" s="18" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="13" t="s">
+      <c r="A69" s="12" t="s">
         <v>285</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B69" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="D69" s="5" t="s">
+      <c r="D69" s="18" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="13" t="s">
+      <c r="A70" s="12" t="s">
         <v>285</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B70" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="D70" s="5" t="s">
+      <c r="D70" s="18" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="13" t="s">
+      <c r="A71" s="12" t="s">
         <v>285</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B71" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C71" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="D71" s="5" t="s">
+      <c r="D71" s="18" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="13" t="s">
+      <c r="A72" s="12" t="s">
         <v>285</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B72" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="C72" t="s">
+      <c r="C72" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="D72" s="5" t="s">
+      <c r="D72" s="18" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="13" t="s">
+      <c r="A73" s="12" t="s">
         <v>285</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B73" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="C73" t="s">
+      <c r="C73" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="D73" s="5" t="s">
+      <c r="D73" s="18" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" s="13" t="s">
+      <c r="A74" s="12" t="s">
         <v>285</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B74" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C74" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="D74" s="5" t="s">
+      <c r="D74" s="18" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" s="13" t="s">
+      <c r="A75" s="12" t="s">
         <v>285</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B75" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C75" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="D75" s="5" t="s">
+      <c r="D75" s="18" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="13" t="s">
+      <c r="A76" s="12" t="s">
         <v>285</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B76" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="C76" t="s">
+      <c r="C76" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="D76" s="5" t="s">
+      <c r="D76" s="18" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" s="13" t="s">
+      <c r="A77" s="12" t="s">
         <v>285</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B77" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="C77" t="s">
+      <c r="C77" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="D77" s="5" t="s">
+      <c r="D77" s="18" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78" s="13" t="s">
+      <c r="A78" s="12" t="s">
         <v>285</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B78" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="C78" t="s">
+      <c r="C78" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="D78" s="5" t="s">
+      <c r="D78" s="18" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B79" t="s">
+      <c r="B79" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="C79" t="s">
+      <c r="C79" s="15" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B80" t="s">
+    <row r="80" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B80" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="C80" s="5" t="s">
+      <c r="C80" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="D80" s="5" t="s">
+      <c r="D80" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="E80" t="s">
+      <c r="E80" s="15" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B81" t="s">
+      <c r="B81" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="C81" s="5" t="s">
+      <c r="C81" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="D81" s="5" t="s">
+      <c r="D81" s="18" t="s">
         <v>116</v>
       </c>
+      <c r="E81" s="15" t="s">
+        <v>289</v>
+      </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B82" t="s">
+      <c r="B82" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="C82" s="5" t="s">
+      <c r="C82" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="D82" s="5" t="s">
+      <c r="D82" s="18" t="s">
         <v>116</v>
       </c>
+      <c r="E82" s="15" t="s">
+        <v>289</v>
+      </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B83" t="s">
+      <c r="B83" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="C83" t="s">
+      <c r="C83" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="D83" s="4" t="s">
+      <c r="D83" s="19" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B84" t="s">
+      <c r="B84" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="C84" s="5" t="s">
+      <c r="C84" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="D84" s="5" t="s">
+      <c r="D84" s="18" t="s">
         <v>116</v>
       </c>
+      <c r="E84" s="15" t="s">
+        <v>289</v>
+      </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B85" t="s">
+      <c r="B85" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="C85" t="s">
+      <c r="C85" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="D85" s="4" t="s">
+      <c r="D85" s="19" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B86" t="s">
+      <c r="B86" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="C86" s="5" t="s">
+      <c r="C86" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="D86" s="5" t="s">
+      <c r="D86" s="18" t="s">
         <v>116</v>
       </c>
+      <c r="E86" s="15" t="s">
+        <v>289</v>
+      </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B87" t="s">
+      <c r="B87" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="C87" t="s">
+      <c r="C87" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="D87" s="4" t="s">
+      <c r="D87" s="19" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B88" t="s">
+      <c r="B88" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="C88" s="5" t="s">
+      <c r="C88" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="D88" s="5" t="s">
+      <c r="D88" s="18" t="s">
         <v>116</v>
       </c>
+      <c r="E88" s="15" t="s">
+        <v>289</v>
+      </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B89" t="s">
+      <c r="B89" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="C89" t="s">
+      <c r="C89" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="D89" s="4" t="s">
+      <c r="D89" s="19" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A90" s="13" t="s">
+      <c r="A90" s="12" t="s">
         <v>285</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B90" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="C90" s="5" t="s">
+      <c r="C90" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="D90" s="5" t="s">
+      <c r="D90" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="E90" t="s">
+      <c r="E90" s="15" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B91" t="s">
+      <c r="B91" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="C91" s="5" t="s">
+      <c r="C91" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="D91" s="5" t="s">
+      <c r="D91" s="18" t="s">
         <v>116</v>
       </c>
+      <c r="E91" s="15" t="s">
+        <v>289</v>
+      </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B92" t="s">
+      <c r="B92" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="C92" t="s">
+      <c r="C92" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="D92" s="4" t="s">
+      <c r="D92" s="19" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B93" t="s">
+      <c r="B93" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="C93" s="5" t="s">
+      <c r="C93" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="D93" s="5" t="s">
+      <c r="D93" s="18" t="s">
         <v>116</v>
       </c>
+      <c r="E93" s="15" t="s">
+        <v>289</v>
+      </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B94" t="s">
+      <c r="B94" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="C94" t="s">
+      <c r="C94" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="D94" s="4" t="s">
+      <c r="D94" s="19" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B95" t="s">
+      <c r="B95" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="C95" s="5" t="s">
+      <c r="C95" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="D95" s="5" t="s">
+      <c r="D95" s="18" t="s">
         <v>116</v>
       </c>
+      <c r="E95" s="15" t="s">
+        <v>289</v>
+      </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B96" t="s">
+      <c r="B96" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="C96" t="s">
+      <c r="C96" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="D96" s="4" t="s">
+      <c r="D96" s="19" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="97" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B97" t="s">
+    <row r="97" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B97" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="C97" s="5" t="s">
+      <c r="C97" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="D97" s="5" t="s">
+      <c r="D97" s="18" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="98" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B98" t="s">
+      <c r="E97" s="15" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="98" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B98" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="C98" s="5" t="s">
+      <c r="C98" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="D98" s="5" t="s">
+      <c r="D98" s="18" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="99" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B99" t="s">
+      <c r="E98" s="15" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="99" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B99" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="C99" s="5" t="s">
+      <c r="C99" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="D99" s="5" t="s">
+      <c r="D99" s="18" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="101" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C101" s="4" t="s">
+      <c r="E99" s="15" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="101" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C101" s="19" t="s">
         <v>165</v>
       </c>
-      <c r="D101" s="4" t="s">
+      <c r="D101" s="19" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="102" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C102" s="4" t="s">
+    <row r="102" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C102" s="19" t="s">
         <v>166</v>
       </c>
-      <c r="D102" s="4" t="s">
+      <c r="D102" s="19" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="103" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C103" s="4" t="s">
+    <row r="103" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C103" s="19" t="s">
         <v>167</v>
       </c>
-      <c r="D103" s="4" t="s">
+      <c r="D103" s="19" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="104" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C104" s="4" t="s">
+    <row r="104" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C104" s="19" t="s">
         <v>168</v>
       </c>
-      <c r="D104" s="4" t="s">
+      <c r="D104" s="19" t="s">
         <v>117</v>
       </c>
     </row>
@@ -2571,875 +2680,889 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3249E01-1138-4B32-9CF1-2F09083F4474}">
-  <dimension ref="B2:E79"/>
+  <dimension ref="B2:F79"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54"/>
+    <sheetView topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="F55" sqref="F55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="81" customWidth="1"/>
-    <col min="3" max="3" width="89" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="89.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="75.42578125" style="15" customWidth="1"/>
+    <col min="3" max="3" width="66.5703125" style="15" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="15"/>
+    <col min="5" max="5" width="53" style="15" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="12" t="s">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="C2" s="12"/>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
+      <c r="C2" s="14"/>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="16" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="16" t="s">
         <v>211</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="16" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+    <row r="5" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B5" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="E5" s="5" t="s">
+      <c r="D5" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="E5" s="18" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="15" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+    <row r="7" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B7" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="19" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="19" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="19" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C10" s="4" t="s">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C10" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="19" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="D11" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="E11" s="15" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
+    <row r="12" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B12" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="E12" t="s">
+      <c r="D12" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="E12" s="15" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="15" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
+    <row r="14" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B14" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="15" t="s">
         <v>231</v>
       </c>
-      <c r="D14" s="5" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
+      <c r="D14" s="18" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B15" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="15" t="s">
         <v>229</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="E15" s="18" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
+      <c r="F15" s="15" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="15" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C18" s="4" t="s">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C18" s="19" t="s">
         <v>279</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="19" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
+    <row r="19" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B19" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="15" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="15" t="s">
         <v>127</v>
       </c>
-      <c r="D20" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="E20" t="s">
+      <c r="D20" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="E20" s="15" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="15" t="s">
         <v>128</v>
       </c>
-      <c r="D21" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="E21" t="s">
+      <c r="D21" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="E21" s="15" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="15" t="s">
         <v>134</v>
       </c>
-      <c r="D22" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="E22" t="s">
+      <c r="D22" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="E22" s="15" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
+    <row r="23" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B23" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="C23" s="18" t="s">
         <v>135</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D23" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="E23" s="5" t="s">
+      <c r="E23" s="18" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
+      <c r="F23" s="20" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B24" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="15" t="s">
         <v>138</v>
       </c>
-      <c r="D24" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="E24" t="s">
+      <c r="D24" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="E24" s="15" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="15" t="s">
         <v>139</v>
       </c>
-      <c r="D25" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="E25" t="s">
+      <c r="D25" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="E25" s="15" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B26" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="15" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B27" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="D27" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="E27" t="s">
+      <c r="D27" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="E27" s="15" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B28" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="15" t="s">
         <v>141</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="D28" s="19" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
+    <row r="29" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B29" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="15" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
+    <row r="30" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B30" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="15" t="s">
         <v>235</v>
       </c>
-      <c r="D30" s="3" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
+      <c r="D30" s="17" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B31" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="15" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B32" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="D32" s="19" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
+    <row r="33" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B33" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="15" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B34" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="15" t="s">
         <v>144</v>
       </c>
-      <c r="D34" s="3" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
+      <c r="D34" s="17" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B35" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" s="15" t="s">
         <v>147</v>
       </c>
-      <c r="D35" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="E35" t="s">
+      <c r="D35" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="E35" s="15" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B36" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="15" t="s">
         <v>148</v>
       </c>
-      <c r="D36" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="E36" t="s">
+      <c r="D36" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="E36" s="15" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
+    <row r="37" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B37" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="15" t="s">
         <v>149</v>
       </c>
-      <c r="D37" s="5" t="s">
+      <c r="D37" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="E37" s="5" t="s">
+      <c r="E37" s="18" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
+      <c r="F37" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B38" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="15" t="s">
         <v>150</v>
       </c>
-      <c r="D38" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="E38" t="s">
+      <c r="D38" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="E38" s="15" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B39" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="D39" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="E39" t="s">
+      <c r="D39" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="E39" s="15" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B40" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C40" s="15" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B41" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41" s="15" t="s">
         <v>152</v>
       </c>
-      <c r="D41" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="E41" t="s">
+      <c r="D41" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="E41" s="15" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B42" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" s="15" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
+    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B43" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C43" s="15" t="s">
         <v>156</v>
       </c>
-      <c r="D43" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="E43" t="s">
+      <c r="D43" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="E43" s="15" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
+    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B44" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44" s="15" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
+    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B45" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C45" s="15" t="s">
         <v>157</v>
       </c>
-      <c r="D45" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="E45" t="s">
+      <c r="D45" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="E45" s="15" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B46" t="s">
+    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B46" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C46" s="15" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
+    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B47" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C47" s="15" t="s">
         <v>158</v>
       </c>
-      <c r="D47" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="E47" t="s">
+      <c r="D47" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="E47" s="15" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B48" t="s">
+    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B48" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C48" s="15" t="s">
         <v>159</v>
       </c>
-      <c r="D48" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="E48" t="s">
+      <c r="D48" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="E48" s="15" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B49" t="s">
+    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B49" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C49" s="15" t="s">
         <v>161</v>
       </c>
-      <c r="D49" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="E49" t="s">
+      <c r="D49" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="E49" s="15" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B50" t="s">
+    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B50" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C50" s="15" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B51" t="s">
+    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B51" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C51" s="15" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B52" t="s">
+    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B52" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C52" s="15" t="s">
         <v>163</v>
       </c>
-      <c r="D52" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="E52" t="s">
+      <c r="D52" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="E52" s="15" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
+    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B53" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C53" s="15" t="s">
         <v>164</v>
       </c>
-      <c r="D53" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="E53" t="s">
+      <c r="D53" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="E53" s="15" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B54" t="s">
+    <row r="54" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B54" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C54" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="D54" s="5" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B55" t="s">
+      <c r="D54" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="F54" s="15" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B55" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C55" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="D55" s="5" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B56" t="s">
+      <c r="D55" s="18" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="56" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B56" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C56" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="D56" s="5" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B57" t="s">
+      <c r="D56" s="18" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B57" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C57" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="D57" s="5" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B58" t="s">
+      <c r="D57" s="18" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="58" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B58" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C58" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="D58" s="5" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="59" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B59" t="s">
+      <c r="D58" s="18" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="59" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B59" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C59" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="D59" s="5" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B60" t="s">
+      <c r="D59" s="18" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="60" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B60" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C60" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="D60" s="5" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B61" t="s">
+      <c r="D60" s="18" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="61" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B61" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C61" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="D61" s="5" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="62" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B62" t="s">
+      <c r="D61" s="18" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="62" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B62" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C62" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="D62" s="5" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B63" t="s">
+      <c r="D62" s="18" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="63" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B63" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C63" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="D63" s="5" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="64" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B64" t="s">
+      <c r="D63" s="18" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="64" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B64" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C64" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="D64" s="5" t="s">
+      <c r="D64" s="18" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B65" t="s">
+      <c r="B65" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C65" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="D65" s="5" t="s">
+      <c r="D65" s="18" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B66" t="s">
+      <c r="B66" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C66" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="D66" s="5" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B67" t="s">
+      <c r="D66" s="18" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="67" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B67" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C67" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="D67" s="5" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="68" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B68" t="s">
+      <c r="D67" s="18" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="68" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B68" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="C68" t="s">
+      <c r="C68" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="D68" s="5" t="s">
+      <c r="D68" s="18" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="69" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B69" t="s">
+      <c r="B69" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="D69" s="5" t="s">
+      <c r="D69" s="18" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="70" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B70" t="s">
+      <c r="B70" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="D70" s="5" t="s">
+      <c r="D70" s="18" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="71" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B71" t="s">
+      <c r="B71" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C71" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="D71" s="5" t="s">
+      <c r="D71" s="18" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="72" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B72" t="s">
+      <c r="B72" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="C72" t="s">
+      <c r="C72" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="D72" s="5" t="s">
+      <c r="D72" s="18" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="73" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B73" t="s">
+      <c r="B73" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="C73" t="s">
+      <c r="C73" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="D73" s="5" t="s">
+      <c r="D73" s="18" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="74" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B74" t="s">
+      <c r="B74" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C74" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="D74" s="5" t="s">
+      <c r="D74" s="18" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="75" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B75" t="s">
+      <c r="B75" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C75" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="D75" s="5" t="s">
+      <c r="D75" s="18" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="76" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B76" t="s">
+      <c r="B76" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="C76" t="s">
+      <c r="C76" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="D76" s="5" t="s">
+      <c r="D76" s="18" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="77" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B77" t="s">
+      <c r="B77" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="C77" t="s">
+      <c r="C77" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="D77" s="5" t="s">
+      <c r="D77" s="18" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="78" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B78" t="s">
+      <c r="B78" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="C78" t="s">
+      <c r="C78" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="D78" s="5" t="s">
+      <c r="D78" s="18" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="79" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B79" t="s">
+      <c r="B79" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="C79" t="s">
+      <c r="C79" s="15" t="s">
         <v>75</v>
       </c>
     </row>
@@ -3456,7 +3579,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7569136C-1755-44CC-8CB8-7F6C3204D25A}">
   <dimension ref="B2:E84"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
+    <sheetView topLeftCell="A52" workbookViewId="0">
       <selection activeCell="C18" sqref="C18:D18"/>
     </sheetView>
   </sheetViews>
@@ -3468,10 +3591,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="13" t="s">
         <v>251</v>
       </c>
-      <c r="C2" s="12"/>
+      <c r="C2" s="13"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
@@ -4390,10 +4513,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4799C5DE-DF6E-46DA-A3CB-E59A285E9DA9}">
-  <dimension ref="B2:E40"/>
+  <dimension ref="B2:F40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18:C18"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4401,16 +4524,16 @@
     <col min="2" max="2" width="57" customWidth="1"/>
     <col min="3" max="3" width="83" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.28515625" customWidth="1"/>
-    <col min="5" max="5" width="89.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="12" t="s">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="13" t="s">
         <v>209</v>
       </c>
-      <c r="C2" s="12"/>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C2" s="13"/>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
@@ -4418,7 +4541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>172</v>
       </c>
@@ -4426,7 +4549,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C5" s="5" t="s">
         <v>189</v>
       </c>
@@ -4436,8 +4559,11 @@
       <c r="E5" s="5" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F5" s="5" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>3</v>
       </c>
@@ -4450,8 +4576,11 @@
       <c r="E6" s="5" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>4</v>
       </c>
@@ -4459,7 +4588,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>13</v>
       </c>
@@ -4467,7 +4596,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>36</v>
       </c>
@@ -4475,7 +4604,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>37</v>
       </c>
@@ -4489,7 +4618,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>39</v>
       </c>
@@ -4503,7 +4632,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>40</v>
       </c>
@@ -4511,7 +4640,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>41</v>
       </c>
@@ -4525,7 +4654,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>42</v>
       </c>
@@ -4533,7 +4662,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>48</v>
       </c>
@@ -4547,7 +4676,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>75</v>
       </c>
@@ -4555,7 +4684,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>173</v>
       </c>
@@ -4569,7 +4698,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>200</v>
       </c>
@@ -4579,8 +4708,11 @@
       <c r="D18" s="5" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F18" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>174</v>
       </c>
@@ -4588,7 +4720,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>175</v>
       </c>
@@ -4596,7 +4728,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>77</v>
       </c>
@@ -4604,7 +4736,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>176</v>
       </c>
@@ -4618,7 +4750,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>177</v>
       </c>
@@ -4632,15 +4764,18 @@
         <v>203</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C24" s="5" t="s">
         <v>281</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F24" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>178</v>
       </c>
@@ -4650,8 +4785,11 @@
       <c r="D25" s="5" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F25" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>78</v>
       </c>
@@ -4659,7 +4797,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>80</v>
       </c>
@@ -4667,7 +4805,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>179</v>
       </c>
@@ -4675,7 +4813,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>36</v>
       </c>
@@ -4683,7 +4821,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>180</v>
       </c>
@@ -4693,8 +4831,11 @@
       <c r="D30" s="5" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F30" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>87</v>
       </c>
@@ -4702,7 +4843,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>181</v>
       </c>
@@ -4710,7 +4851,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>182</v>
       </c>
@@ -4718,7 +4859,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>183</v>
       </c>
@@ -4726,7 +4867,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>184</v>
       </c>
@@ -4734,7 +4875,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>185</v>
       </c>
@@ -4742,7 +4883,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>76</v>
       </c>
@@ -4752,8 +4893,11 @@
       <c r="D37" s="5" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F37" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>186</v>
       </c>
@@ -4761,7 +4905,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>187</v>
       </c>
@@ -4775,7 +4919,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>188</v>
       </c>
@@ -4794,111 +4938,114 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D281CCB-21B2-459E-BC6A-5221B0D209DE}">
-  <dimension ref="B2:E10"/>
+  <dimension ref="B2:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="66.85546875" customWidth="1"/>
-    <col min="3" max="3" width="102.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" customWidth="1"/>
-    <col min="5" max="5" width="89.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="66.85546875" style="15" customWidth="1"/>
+    <col min="3" max="3" width="102.5703125" style="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="15" customWidth="1"/>
+    <col min="5" max="5" width="39.140625" style="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="12" t="s">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="14" t="s">
         <v>171</v>
       </c>
-      <c r="C2" s="12"/>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
+      <c r="C2" s="14"/>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="16" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="16" t="s">
         <v>210</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="16" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="15" t="s">
         <v>215</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="15" t="s">
         <v>213</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="E5" s="3" t="s">
+      <c r="D5" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="E5" s="17" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="15" t="s">
         <v>216</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="15" t="s">
         <v>222</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="E6" s="3" t="s">
+      <c r="D6" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="E6" s="17" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+    <row r="7" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B7" s="15" t="s">
         <v>217</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="15" t="s">
         <v>225</v>
       </c>
-      <c r="D7" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="D7" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="E7" s="15" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+      <c r="F7" s="15" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="15" t="s">
         <v>218</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="15" t="s">
         <v>224</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="19" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="15" t="s">
         <v>219</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="15" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="15" t="s">
         <v>220</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="15" t="s">
         <v>223</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="19" t="s">
         <v>118</v>
       </c>
     </row>
@@ -4915,8 +5062,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9F13751-6B3C-4CAF-8671-2D17A637C6CE}">
   <dimension ref="A2:Q15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9:K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5000,7 +5147,7 @@
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="12" t="s">
         <v>285</v>
       </c>
       <c r="B9" t="s">
@@ -5025,7 +5172,7 @@
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="12" t="s">
         <v>285</v>
       </c>
       <c r="B11" t="s">

</xml_diff>